<commit_message>
bad results for benchmark - wrong graphs for peaks
</commit_message>
<xml_diff>
--- a/ArtigoKrigingVsg/peaks/KrigingMetrics.xlsx
+++ b/ArtigoKrigingVsg/peaks/KrigingMetrics.xlsx
@@ -522,52 +522,52 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.7692941841039236</v>
+        <v>0.7692941849576688</v>
       </c>
       <c r="B2" t="n">
-        <v>1.542730853199666</v>
+        <v>1.542730847490668</v>
       </c>
       <c r="C2" t="n">
-        <v>1.490879223657692</v>
+        <v>1.490879221317486</v>
       </c>
       <c r="D2" t="n">
-        <v>1.242067169359075</v>
+        <v>1.242067167060891</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>3.85602952710407e-30</v>
+        <v>2.075685827223915e-29</v>
       </c>
       <c r="G2" t="n">
-        <v>5.425331801585634e-15</v>
+        <v>1.818878597560449e-14</v>
       </c>
       <c r="H2" t="n">
-        <v>1.963677551713639e-15</v>
+        <v>4.555969520556426e-15</v>
       </c>
       <c r="I2" t="n">
-        <v>0.7739693030189488</v>
+        <v>0.7739693040866447</v>
       </c>
       <c r="J2" t="n">
-        <v>0.8084986970883845</v>
+        <v>0.8084986932692988</v>
       </c>
       <c r="K2" t="n">
-        <v>3.364388917295114</v>
+        <v>3.364388869890441</v>
       </c>
       <c r="L2" t="n">
-        <v>0.8991655559953264</v>
+        <v>0.8991655538716431</v>
       </c>
       <c r="M2" t="n">
-        <v>0.797539898704922</v>
+        <v>0.7819351888578722</v>
       </c>
       <c r="N2" t="n">
-        <v>1.46911667516885</v>
+        <v>1.353359040557771</v>
       </c>
       <c r="O2" t="n">
-        <v>0.8883527418803241</v>
+        <v>0.9574498701462588</v>
       </c>
       <c r="P2" t="n">
-        <v>1.21207123353739</v>
+        <v>1.163339606717562</v>
       </c>
     </row>
   </sheetData>
@@ -673,52 +673,52 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.8276108164108933</v>
+        <v>0.8276108165723453</v>
       </c>
       <c r="B2" t="n">
-        <v>1.152767264439559</v>
+        <v>1.152767263359928</v>
       </c>
       <c r="C2" t="n">
-        <v>1.932715424135034</v>
+        <v>1.93271542165783</v>
       </c>
       <c r="D2" t="n">
-        <v>1.073669997922806</v>
+        <v>1.073669997420031</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>1.304206439750998e-28</v>
+        <v>2.549350771083462e-29</v>
       </c>
       <c r="G2" t="n">
-        <v>2.946859732899593e-14</v>
+        <v>1.9067849121359e-14</v>
       </c>
       <c r="H2" t="n">
-        <v>1.142018581175892e-14</v>
+        <v>5.049109595843074e-15</v>
       </c>
       <c r="I2" t="n">
-        <v>0.8122155034922969</v>
+        <v>0.812215503691748</v>
       </c>
       <c r="J2" t="n">
-        <v>0.6716942556373399</v>
+        <v>0.6716942549239149</v>
       </c>
       <c r="K2" t="n">
-        <v>0.4175751226772103</v>
+        <v>0.4175751219327417</v>
       </c>
       <c r="L2" t="n">
-        <v>0.8195695550942214</v>
+        <v>0.8195695546589776</v>
       </c>
       <c r="M2" t="n">
-        <v>0.8561453234379668</v>
+        <v>0.837852471077039</v>
       </c>
       <c r="N2" t="n">
-        <v>1.043856556360631</v>
+        <v>1.006323867765007</v>
       </c>
       <c r="O2" t="n">
-        <v>0.9862562699817504</v>
+        <v>1.017921705836737</v>
       </c>
       <c r="P2" t="n">
-        <v>1.021692985373116</v>
+        <v>1.0031569507136</v>
       </c>
     </row>
   </sheetData>
@@ -824,52 +824,52 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.7435723845006685</v>
+        <v>0.7435723829541865</v>
       </c>
       <c r="B2" t="n">
-        <v>1.714732645584629</v>
+        <v>1.714732655925962</v>
       </c>
       <c r="C2" t="n">
-        <v>1.319891601556767</v>
+        <v>1.319891597474623</v>
       </c>
       <c r="D2" t="n">
-        <v>1.309478005002233</v>
+        <v>1.30947800895088</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>3.386811362893119e-30</v>
+        <v>1.705243987628719e-29</v>
       </c>
       <c r="G2" t="n">
-        <v>4.903992477118836e-15</v>
+        <v>1.152722558947848e-14</v>
       </c>
       <c r="H2" t="n">
-        <v>1.840329145259923e-15</v>
+        <v>4.129459998145906e-15</v>
       </c>
       <c r="I2" t="n">
-        <v>0.7613785975574645</v>
+        <v>0.7613785966610122</v>
       </c>
       <c r="J2" t="n">
-        <v>0.8535349204730651</v>
+        <v>0.8535349236796232</v>
       </c>
       <c r="K2" t="n">
-        <v>3.48302650381743</v>
+        <v>3.483026505441671</v>
       </c>
       <c r="L2" t="n">
-        <v>0.9238695365001841</v>
+        <v>0.9238695382355797</v>
       </c>
       <c r="M2" t="n">
-        <v>0.7690054573958218</v>
+        <v>0.7554879657324924</v>
       </c>
       <c r="N2" t="n">
-        <v>1.676171908647809</v>
+        <v>1.517496428552264</v>
       </c>
       <c r="O2" t="n">
-        <v>0.7122811875347786</v>
+        <v>0.796816168213166</v>
       </c>
       <c r="P2" t="n">
-        <v>1.294670579200674</v>
+        <v>1.23186704986872</v>
       </c>
     </row>
   </sheetData>
@@ -975,52 +975,52 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.2813534340745442</v>
+        <v>0.2813534431453613</v>
       </c>
       <c r="B2" t="n">
-        <v>4.80559289540669</v>
+        <v>4.805592834750094</v>
       </c>
       <c r="C2" t="n">
-        <v>1.732046163950706</v>
+        <v>1.732046185857099</v>
       </c>
       <c r="D2" t="n">
-        <v>2.192166256333376</v>
+        <v>2.192166242498523</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>2.334159685049276e-30</v>
+        <v>2.009116636475154e-30</v>
       </c>
       <c r="G2" t="n">
-        <v>3.781302281937423e-15</v>
+        <v>3.955089848909272e-15</v>
       </c>
       <c r="H2" t="n">
-        <v>1.527795694799955e-15</v>
+        <v>1.417433115344478e-15</v>
       </c>
       <c r="I2" t="n">
-        <v>0.3845846744856987</v>
+        <v>0.3845846849934301</v>
       </c>
       <c r="J2" t="n">
-        <v>2.201304935533818</v>
+        <v>2.201304897948272</v>
       </c>
       <c r="K2" t="n">
-        <v>4.455349773514302</v>
+        <v>4.455349818907312</v>
       </c>
       <c r="L2" t="n">
-        <v>1.483679525886173</v>
+        <v>1.483679513219843</v>
       </c>
       <c r="M2" t="n">
-        <v>0.3010598466482847</v>
+        <v>0.2974918202433614</v>
       </c>
       <c r="N2" t="n">
-        <v>5.071738222325199</v>
+        <v>4.359923048381081</v>
       </c>
       <c r="O2" t="n">
-        <v>2.981893333037033</v>
+        <v>2.664742142868901</v>
       </c>
       <c r="P2" t="n">
-        <v>2.252052002580136</v>
+        <v>2.088042875129982</v>
       </c>
     </row>
   </sheetData>
@@ -1126,52 +1126,52 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.5477659651296473</v>
+        <v>0.5477659675530802</v>
       </c>
       <c r="B2" t="n">
-        <v>3.024091073524307</v>
+        <v>3.0240910573188</v>
       </c>
       <c r="C2" t="n">
-        <v>1.687083468132193</v>
+        <v>1.687083469284017</v>
       </c>
       <c r="D2" t="n">
-        <v>1.738991395471613</v>
+        <v>1.738991390812157</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>3.265215849924287e-30</v>
+        <v>3.874062009173368e-30</v>
       </c>
       <c r="G2" t="n">
-        <v>5.977925339076233e-15</v>
+        <v>5.612399192364684e-15</v>
       </c>
       <c r="H2" t="n">
-        <v>1.806990827293898e-15</v>
+        <v>1.968263704175172e-15</v>
       </c>
       <c r="I2" t="n">
-        <v>0.6136626822785356</v>
+        <v>0.613662684371109</v>
       </c>
       <c r="J2" t="n">
-        <v>1.381906184364909</v>
+        <v>1.381906176879894</v>
       </c>
       <c r="K2" t="n">
-        <v>4.770316124543085</v>
+        <v>4.770316126117107</v>
       </c>
       <c r="L2" t="n">
-        <v>1.175545058415418</v>
+        <v>1.175545055231782</v>
       </c>
       <c r="M2" t="n">
-        <v>0.5635475798666887</v>
+        <v>0.5543866075244759</v>
       </c>
       <c r="N2" t="n">
-        <v>3.167041428084265</v>
+        <v>2.765576482247305</v>
       </c>
       <c r="O2" t="n">
-        <v>1.937724142947162</v>
+        <v>1.814180411310868</v>
       </c>
       <c r="P2" t="n">
-        <v>1.779618337757921</v>
+        <v>1.663002249621841</v>
       </c>
     </row>
   </sheetData>
@@ -1277,52 +1277,52 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.005407713594795638</v>
+        <v>-0.005407713470203523</v>
       </c>
       <c r="B2" t="n">
-        <v>6.723166010285237</v>
+        <v>6.723166009452089</v>
       </c>
       <c r="C2" t="n">
-        <v>2.063041572457557</v>
+        <v>2.063041572240144</v>
       </c>
       <c r="D2" t="n">
-        <v>2.59290686494622</v>
+        <v>2.592906864785561</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>1.068559088812504e-29</v>
+        <v>6.423361550520309e-30</v>
       </c>
       <c r="G2" t="n">
-        <v>1.164438802135919e-14</v>
+        <v>8.227612281004692e-15</v>
       </c>
       <c r="H2" t="n">
-        <v>3.268882207747021e-15</v>
+        <v>2.534435154135988e-15</v>
       </c>
       <c r="I2" t="n">
-        <v>0.01501071341073634</v>
+        <v>0.01501071341073656</v>
       </c>
       <c r="J2" t="n">
-        <v>3.523249565169454</v>
+        <v>3.523249565169453</v>
       </c>
       <c r="K2" t="n">
-        <v>3.21235751683888</v>
+        <v>3.212357516838896</v>
       </c>
       <c r="L2" t="n">
         <v>1.877032116179543</v>
       </c>
       <c r="M2" t="n">
-        <v>-0.00268611410671582</v>
+        <v>-0.001948746461204243</v>
       </c>
       <c r="N2" t="n">
-        <v>7.275818202063919</v>
+        <v>6.218318247206794</v>
       </c>
       <c r="O2" t="n">
-        <v>2.947450498018319</v>
+        <v>2.590983844690503</v>
       </c>
       <c r="P2" t="n">
-        <v>2.697372462613185</v>
+        <v>2.493655599156947</v>
       </c>
     </row>
   </sheetData>

</xml_diff>